<commit_message>
video call with local video not being able to see
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DevX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CAC3579-1CEB-4382-AF96-5CEF4F3061E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C84FE6-3367-41E7-BC02-EC0E44F48AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7560" windowWidth="29040" windowHeight="15720" xr2:uid="{59A5B4B3-141C-44D1-8862-EE0E02C6293A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{59A5B4B3-141C-44D1-8862-EE0E02C6293A}"/>
   </bookViews>
   <sheets>
     <sheet name="URA" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="528">
   <si>
     <t>Req. Code</t>
   </si>
@@ -510,9 +510,6 @@
     <t>Application UI should adapt to different screen size without any loss of functionality and usability.</t>
   </si>
   <si>
-    <t>UI testing</t>
-  </si>
-  <si>
     <t>JRS-F-1.0</t>
   </si>
   <si>
@@ -711,9 +708,6 @@
     <t>Top 3 jobs with highest cosine similarity scores are recommended.</t>
   </si>
   <si>
-    <t>N configurable</t>
-  </si>
-  <si>
     <t>TC-JRS-F-1.8_017</t>
   </si>
   <si>
@@ -912,9 +906,6 @@
     <t>Job posting is stored in the database successfully.</t>
   </si>
   <si>
-    <t>Need DB Access</t>
-  </si>
-  <si>
     <t>JMS-UR-1.7</t>
   </si>
   <si>
@@ -1621,6 +1612,18 @@
   </si>
   <si>
     <t>System throws an error that the message cannot be deleted as the time to delete the message has lapsed.</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skill extraction needs to be better </t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
@@ -1673,10 +1676,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1998,8 +1997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A82B2ACD-BE2D-4DD6-B6CD-A58F7A0DD893}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2049,6 +2048,9 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
+      <c r="F2" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -2066,6 +2068,9 @@
       <c r="E3" t="s">
         <v>16</v>
       </c>
+      <c r="F3" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -2083,6 +2088,9 @@
       <c r="E4" t="s">
         <v>21</v>
       </c>
+      <c r="F4" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -2100,6 +2108,9 @@
       <c r="E5" t="s">
         <v>24</v>
       </c>
+      <c r="F5" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -2117,6 +2128,9 @@
       <c r="E6" t="s">
         <v>29</v>
       </c>
+      <c r="F6" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -2134,6 +2148,9 @@
       <c r="E7" t="s">
         <v>32</v>
       </c>
+      <c r="F7" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -2151,6 +2168,9 @@
       <c r="E8" t="s">
         <v>37</v>
       </c>
+      <c r="F8" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -2168,6 +2188,9 @@
       <c r="E9" t="s">
         <v>40</v>
       </c>
+      <c r="F9" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -2185,6 +2208,9 @@
       <c r="E10" t="s">
         <v>45</v>
       </c>
+      <c r="F10" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -2202,6 +2228,9 @@
       <c r="E11" t="s">
         <v>50</v>
       </c>
+      <c r="F11" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -2219,6 +2248,9 @@
       <c r="E12" t="s">
         <v>55</v>
       </c>
+      <c r="F12" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -2236,6 +2268,9 @@
       <c r="E13" t="s">
         <v>60</v>
       </c>
+      <c r="F13" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -2253,6 +2288,9 @@
       <c r="E14" t="s">
         <v>65</v>
       </c>
+      <c r="F14" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -2270,6 +2308,9 @@
       <c r="E15" t="s">
         <v>70</v>
       </c>
+      <c r="F15" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -2287,8 +2328,11 @@
       <c r="E16" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -2304,8 +2348,11 @@
       <c r="E17" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>81</v>
       </c>
@@ -2321,8 +2368,11 @@
       <c r="E18" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>86</v>
       </c>
@@ -2338,8 +2388,11 @@
       <c r="E19" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -2355,8 +2408,11 @@
       <c r="E20" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>96</v>
       </c>
@@ -2372,8 +2428,11 @@
       <c r="E21" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>101</v>
       </c>
@@ -2389,8 +2448,11 @@
       <c r="E22" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>106</v>
       </c>
@@ -2406,8 +2468,11 @@
       <c r="E23" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>111</v>
       </c>
@@ -2423,8 +2488,11 @@
       <c r="E24" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>116</v>
       </c>
@@ -2440,8 +2508,11 @@
       <c r="E25" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>121</v>
       </c>
@@ -2457,8 +2528,11 @@
       <c r="E26" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F26" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>126</v>
       </c>
@@ -2474,8 +2548,11 @@
       <c r="E27" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>131</v>
       </c>
@@ -2491,8 +2568,11 @@
       <c r="E28" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F28" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>136</v>
       </c>
@@ -2508,8 +2588,11 @@
       <c r="E29" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F29" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>141</v>
       </c>
@@ -2525,8 +2608,11 @@
       <c r="E30" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F30" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>146</v>
       </c>
@@ -2542,8 +2628,11 @@
       <c r="E31" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F31" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>151</v>
       </c>
@@ -2558,6 +2647,9 @@
       </c>
       <c r="E32" t="s">
         <v>155</v>
+      </c>
+      <c r="F32" t="s">
+        <v>524</v>
       </c>
     </row>
   </sheetData>
@@ -2569,19 +2661,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFA6035C-C709-47DF-9566-B093F753E5EF}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection sqref="A1:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="161.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="148.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="85" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="88.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="77.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="81.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -2609,368 +2701,425 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" t="s">
         <v>157</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>158</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>159</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>160</v>
       </c>
-      <c r="E2" t="s">
-        <v>161</v>
+      <c r="F2" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" t="s">
         <v>157</v>
       </c>
-      <c r="B3" t="s">
-        <v>158</v>
-      </c>
       <c r="C3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D3" t="s">
         <v>162</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>163</v>
       </c>
-      <c r="E3" t="s">
-        <v>164</v>
+      <c r="F3" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" t="s">
         <v>165</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>166</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>167</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>168</v>
       </c>
-      <c r="E4" t="s">
-        <v>169</v>
+      <c r="F4" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" t="s">
         <v>165</v>
       </c>
-      <c r="B5" t="s">
-        <v>166</v>
-      </c>
       <c r="C5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D5" t="s">
         <v>170</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>171</v>
       </c>
-      <c r="E5" t="s">
-        <v>172</v>
+      <c r="F5" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6" t="s">
         <v>173</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>174</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>175</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>176</v>
       </c>
-      <c r="E6" t="s">
-        <v>177</v>
+      <c r="F6" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B7" t="s">
         <v>173</v>
       </c>
-      <c r="B7" t="s">
-        <v>174</v>
-      </c>
       <c r="C7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D7" t="s">
         <v>178</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>179</v>
       </c>
-      <c r="E7" t="s">
-        <v>180</v>
+      <c r="F7" t="s">
+        <v>525</v>
+      </c>
+      <c r="G7" t="s">
+        <v>526</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B8" t="s">
         <v>181</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>182</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>183</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>184</v>
       </c>
-      <c r="E8" t="s">
-        <v>185</v>
+      <c r="F8" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B9" t="s">
         <v>181</v>
       </c>
-      <c r="B9" t="s">
-        <v>182</v>
-      </c>
       <c r="C9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D9" t="s">
         <v>186</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>187</v>
       </c>
-      <c r="E9" t="s">
-        <v>188</v>
+      <c r="F9" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B10" t="s">
         <v>189</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>190</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>191</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>192</v>
       </c>
-      <c r="E10" t="s">
-        <v>193</v>
+      <c r="F10" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" t="s">
         <v>189</v>
       </c>
-      <c r="B11" t="s">
-        <v>190</v>
-      </c>
       <c r="C11" t="s">
+        <v>193</v>
+      </c>
+      <c r="D11" t="s">
         <v>194</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>195</v>
       </c>
-      <c r="E11" t="s">
-        <v>196</v>
+      <c r="F11" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>196</v>
+      </c>
+      <c r="B12" t="s">
         <v>197</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>198</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>199</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>200</v>
       </c>
-      <c r="E12" t="s">
-        <v>201</v>
+      <c r="F12" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>196</v>
+      </c>
+      <c r="B13" t="s">
         <v>197</v>
       </c>
-      <c r="B13" t="s">
-        <v>198</v>
-      </c>
       <c r="C13" t="s">
+        <v>201</v>
+      </c>
+      <c r="D13" t="s">
         <v>202</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>203</v>
       </c>
-      <c r="E13" t="s">
-        <v>204</v>
+      <c r="F13" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>204</v>
+      </c>
+      <c r="B14" t="s">
         <v>205</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>206</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>207</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>208</v>
       </c>
-      <c r="E14" t="s">
-        <v>209</v>
+      <c r="F14" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>204</v>
+      </c>
+      <c r="B15" t="s">
         <v>205</v>
       </c>
-      <c r="B15" t="s">
-        <v>206</v>
-      </c>
       <c r="C15" t="s">
+        <v>209</v>
+      </c>
+      <c r="D15" t="s">
         <v>210</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>211</v>
       </c>
-      <c r="E15" t="s">
-        <v>212</v>
+      <c r="F15" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>212</v>
+      </c>
+      <c r="B16" t="s">
         <v>213</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>214</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>215</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>216</v>
       </c>
-      <c r="E16" t="s">
-        <v>217</v>
+      <c r="F16" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>217</v>
+      </c>
+      <c r="B17" t="s">
         <v>218</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>219</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>220</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>221</v>
       </c>
-      <c r="E17" t="s">
-        <v>222</v>
-      </c>
       <c r="F17" t="s">
-        <v>223</v>
+        <v>524</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>217</v>
+      </c>
+      <c r="B18" t="s">
         <v>218</v>
       </c>
-      <c r="B18" t="s">
-        <v>219</v>
-      </c>
       <c r="C18" t="s">
+        <v>222</v>
+      </c>
+      <c r="D18" t="s">
+        <v>223</v>
+      </c>
+      <c r="E18" t="s">
         <v>224</v>
       </c>
-      <c r="D18" t="s">
-        <v>225</v>
-      </c>
-      <c r="E18" t="s">
-        <v>226</v>
-      </c>
       <c r="F18" t="s">
-        <v>223</v>
+        <v>524</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>225</v>
+      </c>
+      <c r="B19" t="s">
+        <v>226</v>
+      </c>
+      <c r="C19" t="s">
         <v>227</v>
       </c>
-      <c r="B19" t="s">
+      <c r="D19" t="s">
         <v>228</v>
       </c>
-      <c r="C19" t="s">
+      <c r="E19" t="s">
         <v>229</v>
       </c>
-      <c r="D19" t="s">
-        <v>230</v>
-      </c>
-      <c r="E19" t="s">
-        <v>231</v>
+      <c r="F19" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B20" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C20" t="s">
+        <v>230</v>
+      </c>
+      <c r="D20" t="s">
+        <v>231</v>
+      </c>
+      <c r="E20" t="s">
         <v>232</v>
       </c>
-      <c r="D20" t="s">
-        <v>233</v>
-      </c>
-      <c r="E20" t="s">
-        <v>234</v>
-      </c>
       <c r="F20" t="s">
-        <v>156</v>
+        <v>524</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>233</v>
+      </c>
+      <c r="B21" t="s">
+        <v>234</v>
+      </c>
+      <c r="C21" t="s">
         <v>235</v>
       </c>
-      <c r="B21" t="s">
+      <c r="D21" t="s">
         <v>236</v>
       </c>
-      <c r="C21" t="s">
+      <c r="E21" t="s">
         <v>237</v>
       </c>
-      <c r="D21" t="s">
-        <v>238</v>
-      </c>
-      <c r="E21" t="s">
-        <v>239</v>
+      <c r="F21" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B22" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C22" t="s">
+        <v>238</v>
+      </c>
+      <c r="D22" t="s">
+        <v>239</v>
+      </c>
+      <c r="E22" t="s">
         <v>240</v>
       </c>
-      <c r="D22" t="s">
-        <v>241</v>
-      </c>
-      <c r="E22" t="s">
-        <v>242</v>
+      <c r="F22" t="s">
+        <v>524</v>
       </c>
     </row>
   </sheetData>
@@ -2982,8 +3131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37FA9BA1-21F1-4D09-B646-2F5EB271BAF0}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3022,589 +3171,682 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C2" t="s">
         <v>243</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>244</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>245</v>
       </c>
-      <c r="D2" t="s">
-        <v>246</v>
-      </c>
-      <c r="E2" t="s">
-        <v>247</v>
+      <c r="F2" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E3" t="s">
         <v>248</v>
       </c>
-      <c r="D3" t="s">
-        <v>249</v>
-      </c>
-      <c r="E3" t="s">
-        <v>250</v>
+      <c r="F3" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B4" t="s">
+        <v>250</v>
+      </c>
+      <c r="C4" t="s">
         <v>251</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>252</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>253</v>
       </c>
-      <c r="D4" t="s">
-        <v>254</v>
-      </c>
-      <c r="E4" t="s">
-        <v>255</v>
+      <c r="F4" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C5" t="s">
+        <v>254</v>
+      </c>
+      <c r="D5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E5" t="s">
         <v>256</v>
       </c>
-      <c r="D5" t="s">
-        <v>257</v>
-      </c>
-      <c r="E5" t="s">
-        <v>258</v>
+      <c r="F5" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>257</v>
+      </c>
+      <c r="B6" t="s">
+        <v>258</v>
+      </c>
+      <c r="C6" t="s">
         <v>259</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>260</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>261</v>
       </c>
-      <c r="D6" t="s">
-        <v>262</v>
-      </c>
-      <c r="E6" t="s">
-        <v>263</v>
+      <c r="F6" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B7" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C7" t="s">
+        <v>262</v>
+      </c>
+      <c r="D7" t="s">
+        <v>263</v>
+      </c>
+      <c r="E7" t="s">
         <v>264</v>
       </c>
-      <c r="D7" t="s">
-        <v>265</v>
-      </c>
-      <c r="E7" t="s">
-        <v>266</v>
+      <c r="F7" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>265</v>
+      </c>
+      <c r="B8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C8" t="s">
         <v>267</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>268</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>269</v>
       </c>
-      <c r="D8" t="s">
-        <v>270</v>
-      </c>
-      <c r="E8" t="s">
-        <v>271</v>
+      <c r="F8" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>270</v>
+      </c>
+      <c r="B9" t="s">
+        <v>271</v>
+      </c>
+      <c r="C9" t="s">
         <v>272</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>273</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>274</v>
       </c>
-      <c r="D9" t="s">
-        <v>275</v>
-      </c>
-      <c r="E9" t="s">
-        <v>276</v>
+      <c r="F9" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B10" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C10" t="s">
+        <v>275</v>
+      </c>
+      <c r="D10" t="s">
+        <v>276</v>
+      </c>
+      <c r="E10" t="s">
         <v>277</v>
       </c>
-      <c r="D10" t="s">
-        <v>278</v>
-      </c>
-      <c r="E10" t="s">
-        <v>279</v>
+      <c r="F10" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>278</v>
+      </c>
+      <c r="B11" t="s">
+        <v>279</v>
+      </c>
+      <c r="C11" t="s">
         <v>280</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
         <v>281</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
         <v>282</v>
       </c>
-      <c r="D11" t="s">
-        <v>283</v>
-      </c>
-      <c r="E11" t="s">
-        <v>284</v>
+      <c r="F11" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>283</v>
+      </c>
+      <c r="B12" t="s">
+        <v>284</v>
+      </c>
+      <c r="C12" t="s">
         <v>285</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
         <v>286</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>287</v>
       </c>
-      <c r="D12" t="s">
-        <v>288</v>
-      </c>
-      <c r="E12" t="s">
-        <v>289</v>
-      </c>
       <c r="F12" t="s">
-        <v>290</v>
+        <v>524</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>288</v>
+      </c>
+      <c r="B13" t="s">
+        <v>289</v>
+      </c>
+      <c r="C13" t="s">
+        <v>290</v>
+      </c>
+      <c r="D13" t="s">
         <v>291</v>
       </c>
-      <c r="B13" t="s">
+      <c r="E13" t="s">
         <v>292</v>
       </c>
-      <c r="C13" t="s">
-        <v>293</v>
-      </c>
-      <c r="D13" t="s">
-        <v>294</v>
-      </c>
-      <c r="E13" t="s">
-        <v>295</v>
-      </c>
       <c r="F13" t="s">
-        <v>156</v>
+        <v>524</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>293</v>
+      </c>
+      <c r="B14" t="s">
+        <v>294</v>
+      </c>
+      <c r="C14" t="s">
+        <v>295</v>
+      </c>
+      <c r="D14" t="s">
         <v>296</v>
       </c>
-      <c r="B14" t="s">
+      <c r="E14" t="s">
         <v>297</v>
       </c>
-      <c r="C14" t="s">
-        <v>298</v>
-      </c>
-      <c r="D14" t="s">
-        <v>299</v>
-      </c>
-      <c r="E14" t="s">
-        <v>300</v>
+      <c r="F14" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B15" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C15" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D15" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="E15" t="s">
-        <v>303</v>
+        <v>300</v>
+      </c>
+      <c r="F15" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B16" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C16" t="s">
+        <v>301</v>
+      </c>
+      <c r="D16" t="s">
+        <v>302</v>
+      </c>
+      <c r="E16" t="s">
+        <v>303</v>
+      </c>
+      <c r="F16" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>304</v>
       </c>
-      <c r="D16" t="s">
+      <c r="B17" t="s">
         <v>305</v>
       </c>
-      <c r="E16" t="s">
+      <c r="C17" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="D17" t="s">
         <v>307</v>
       </c>
-      <c r="B17" t="s">
+      <c r="E17" t="s">
         <v>308</v>
       </c>
-      <c r="C17" t="s">
+      <c r="F17" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>309</v>
       </c>
-      <c r="D17" t="s">
+      <c r="B18" t="s">
         <v>310</v>
       </c>
-      <c r="E17" t="s">
+      <c r="C18" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="D18" t="s">
         <v>312</v>
       </c>
-      <c r="B18" t="s">
+      <c r="E18" t="s">
         <v>313</v>
       </c>
-      <c r="C18" t="s">
+      <c r="F18" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>309</v>
+      </c>
+      <c r="B19" t="s">
+        <v>310</v>
+      </c>
+      <c r="C19" t="s">
         <v>314</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>315</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" t="s">
+        <v>264</v>
+      </c>
+      <c r="F19" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>312</v>
-      </c>
-      <c r="B19" t="s">
-        <v>313</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B20" t="s">
         <v>317</v>
       </c>
-      <c r="D19" t="s">
+      <c r="C20" t="s">
         <v>318</v>
       </c>
-      <c r="E19" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="D20" t="s">
         <v>319</v>
       </c>
-      <c r="B20" t="s">
+      <c r="E20" t="s">
         <v>320</v>
       </c>
-      <c r="C20" t="s">
+      <c r="F20" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>316</v>
+      </c>
+      <c r="B21" t="s">
+        <v>317</v>
+      </c>
+      <c r="C21" t="s">
         <v>321</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>322</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E21" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>319</v>
-      </c>
-      <c r="B21" t="s">
-        <v>320</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="F21" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>324</v>
       </c>
-      <c r="D21" t="s">
+      <c r="B22" t="s">
         <v>325</v>
       </c>
-      <c r="E21" t="s">
+      <c r="C22" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="D22" t="s">
         <v>327</v>
       </c>
-      <c r="B22" t="s">
+      <c r="E22" t="s">
         <v>328</v>
       </c>
-      <c r="C22" t="s">
+      <c r="F22" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>329</v>
       </c>
-      <c r="D22" t="s">
+      <c r="B23" t="s">
         <v>330</v>
       </c>
-      <c r="E22" t="s">
+      <c r="C23" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="D23" t="s">
         <v>332</v>
       </c>
-      <c r="B23" t="s">
+      <c r="E23" t="s">
         <v>333</v>
       </c>
-      <c r="C23" t="s">
+      <c r="F23" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>329</v>
+      </c>
+      <c r="B24" t="s">
+        <v>330</v>
+      </c>
+      <c r="C24" t="s">
         <v>334</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>335</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>332</v>
-      </c>
-      <c r="B24" t="s">
-        <v>333</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="F24" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>337</v>
       </c>
-      <c r="D24" t="s">
+      <c r="B25" t="s">
         <v>338</v>
       </c>
-      <c r="E24" t="s">
+      <c r="C25" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="D25" t="s">
         <v>340</v>
       </c>
-      <c r="B25" t="s">
+      <c r="E25" t="s">
         <v>341</v>
       </c>
-      <c r="C25" t="s">
+      <c r="F25" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>342</v>
       </c>
-      <c r="D25" t="s">
+      <c r="B26" t="s">
         <v>343</v>
       </c>
-      <c r="E25" t="s">
+      <c r="C26" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="D26" t="s">
         <v>345</v>
       </c>
-      <c r="B26" t="s">
+      <c r="E26" t="s">
         <v>346</v>
       </c>
-      <c r="C26" t="s">
+      <c r="F26" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>347</v>
       </c>
-      <c r="D26" t="s">
+      <c r="B27" t="s">
         <v>348</v>
       </c>
-      <c r="E26" t="s">
+      <c r="C27" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="D27" t="s">
         <v>350</v>
       </c>
-      <c r="B27" t="s">
+      <c r="E27" t="s">
         <v>351</v>
       </c>
-      <c r="C27" t="s">
+      <c r="F27" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>352</v>
       </c>
-      <c r="D27" t="s">
+      <c r="B28" t="s">
         <v>353</v>
       </c>
-      <c r="E27" t="s">
+      <c r="C28" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="D28" t="s">
         <v>355</v>
       </c>
-      <c r="B28" t="s">
+      <c r="E28" t="s">
         <v>356</v>
       </c>
-      <c r="C28" t="s">
+      <c r="F28" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>357</v>
       </c>
-      <c r="D28" t="s">
+      <c r="B29" t="s">
         <v>358</v>
       </c>
-      <c r="E28" t="s">
+      <c r="C29" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="D29" t="s">
         <v>360</v>
       </c>
-      <c r="B29" t="s">
+      <c r="E29" t="s">
         <v>361</v>
       </c>
-      <c r="C29" t="s">
+      <c r="F29" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>357</v>
+      </c>
+      <c r="B30" t="s">
         <v>362</v>
       </c>
-      <c r="D29" t="s">
+      <c r="C30" t="s">
         <v>363</v>
       </c>
-      <c r="E29" t="s">
+      <c r="D30" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>360</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="E30" t="s">
         <v>365</v>
       </c>
-      <c r="C30" t="s">
+      <c r="F30" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>366</v>
       </c>
-      <c r="D30" t="s">
+      <c r="B31" t="s">
         <v>367</v>
       </c>
-      <c r="E30" t="s">
+      <c r="C31" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="D31" t="s">
         <v>369</v>
       </c>
-      <c r="B31" t="s">
+      <c r="E31" t="s">
         <v>370</v>
       </c>
-      <c r="C31" t="s">
+      <c r="F31" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>371</v>
       </c>
-      <c r="D31" t="s">
+      <c r="B32" t="s">
         <v>372</v>
       </c>
-      <c r="E31" t="s">
+      <c r="C32" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="D32" t="s">
         <v>374</v>
       </c>
-      <c r="B32" t="s">
+      <c r="E32" t="s">
         <v>375</v>
       </c>
-      <c r="C32" t="s">
-        <v>376</v>
-      </c>
-      <c r="D32" t="s">
-        <v>377</v>
-      </c>
-      <c r="E32" t="s">
-        <v>378</v>
+      <c r="F32" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>376</v>
+      </c>
+      <c r="B33" t="s">
+        <v>377</v>
+      </c>
+      <c r="C33" t="s">
+        <v>378</v>
+      </c>
+      <c r="D33" t="s">
         <v>379</v>
       </c>
-      <c r="B33" t="s">
+      <c r="E33" t="s">
         <v>380</v>
       </c>
-      <c r="C33" t="s">
-        <v>381</v>
-      </c>
-      <c r="D33" t="s">
-        <v>382</v>
-      </c>
-      <c r="E33" t="s">
-        <v>383</v>
-      </c>
       <c r="F33" t="s">
-        <v>290</v>
+        <v>524</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>381</v>
+      </c>
+      <c r="B34" t="s">
+        <v>382</v>
+      </c>
+      <c r="C34" t="s">
+        <v>383</v>
+      </c>
+      <c r="D34" t="s">
         <v>384</v>
       </c>
-      <c r="B34" t="s">
+      <c r="E34" t="s">
         <v>385</v>
       </c>
-      <c r="C34" t="s">
-        <v>386</v>
-      </c>
-      <c r="D34" t="s">
-        <v>387</v>
-      </c>
-      <c r="E34" t="s">
-        <v>388</v>
+      <c r="F34" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B35" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C35" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D35" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="E35" t="s">
-        <v>391</v>
+        <v>388</v>
+      </c>
+      <c r="F35" t="s">
+        <v>524</v>
       </c>
     </row>
   </sheetData>
@@ -3614,10 +3856,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DACA8657-FFE4-4591-8953-EEC382E37854}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3631,7 +3873,7 @@
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3650,280 +3892,325 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B2" t="s">
+        <v>390</v>
+      </c>
+      <c r="C2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D2" t="s">
         <v>392</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>393</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>389</v>
+      </c>
+      <c r="B3" t="s">
+        <v>390</v>
+      </c>
+      <c r="C3" t="s">
         <v>394</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>395</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>392</v>
-      </c>
-      <c r="B3" t="s">
-        <v>393</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>397</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B4" t="s">
         <v>398</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C4" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="D4" t="s">
         <v>400</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>401</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>397</v>
+      </c>
+      <c r="B5" t="s">
+        <v>398</v>
+      </c>
+      <c r="C5" t="s">
         <v>402</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>403</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>400</v>
-      </c>
-      <c r="B5" t="s">
-        <v>401</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="F5" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>397</v>
+      </c>
+      <c r="B6" t="s">
+        <v>398</v>
+      </c>
+      <c r="C6" t="s">
         <v>405</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>406</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>400</v>
-      </c>
-      <c r="B6" t="s">
-        <v>401</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="F6" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>408</v>
       </c>
-      <c r="D6" t="s">
+      <c r="B7" t="s">
         <v>409</v>
       </c>
-      <c r="E6" t="s">
+      <c r="C7" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="D7" t="s">
         <v>411</v>
       </c>
-      <c r="B7" t="s">
+      <c r="E7" t="s">
         <v>412</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F7" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>413</v>
       </c>
-      <c r="D7" t="s">
+      <c r="B8" t="s">
         <v>414</v>
       </c>
-      <c r="E7" t="s">
+      <c r="C8" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="D8" t="s">
         <v>416</v>
       </c>
-      <c r="B8" t="s">
+      <c r="E8" t="s">
         <v>417</v>
       </c>
-      <c r="C8" t="s">
+      <c r="F8" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>418</v>
       </c>
-      <c r="D8" t="s">
+      <c r="B9" t="s">
         <v>419</v>
       </c>
-      <c r="E8" t="s">
+      <c r="C9" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="D9" t="s">
         <v>421</v>
       </c>
-      <c r="B9" t="s">
+      <c r="E9" t="s">
         <v>422</v>
       </c>
-      <c r="C9" t="s">
+      <c r="F9" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>418</v>
+      </c>
+      <c r="B10" t="s">
+        <v>419</v>
+      </c>
+      <c r="C10" t="s">
         <v>423</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>424</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>421</v>
-      </c>
-      <c r="B10" t="s">
-        <v>422</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="F10" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>426</v>
       </c>
-      <c r="D10" t="s">
+      <c r="B11" t="s">
         <v>427</v>
       </c>
-      <c r="E10" t="s">
+      <c r="C11" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="D11" t="s">
         <v>429</v>
       </c>
-      <c r="B11" t="s">
+      <c r="E11" t="s">
         <v>430</v>
       </c>
-      <c r="C11" t="s">
+      <c r="F11" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>426</v>
+      </c>
+      <c r="B12" t="s">
+        <v>427</v>
+      </c>
+      <c r="C12" t="s">
         <v>431</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>432</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>429</v>
-      </c>
-      <c r="B12" t="s">
-        <v>430</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="F12" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>434</v>
       </c>
-      <c r="D12" t="s">
+      <c r="B13" t="s">
         <v>435</v>
       </c>
-      <c r="E12" t="s">
+      <c r="C13" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="D13" t="s">
         <v>437</v>
       </c>
-      <c r="B13" t="s">
+      <c r="E13" t="s">
         <v>438</v>
       </c>
-      <c r="C13" t="s">
+      <c r="F13" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>439</v>
       </c>
-      <c r="D13" t="s">
+      <c r="B14" t="s">
         <v>440</v>
       </c>
-      <c r="E13" t="s">
+      <c r="C14" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="D14" t="s">
         <v>442</v>
       </c>
-      <c r="B14" t="s">
+      <c r="E14" t="s">
         <v>443</v>
       </c>
-      <c r="C14" t="s">
+      <c r="F14" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>444</v>
       </c>
-      <c r="D14" t="s">
+      <c r="B15" t="s">
         <v>445</v>
       </c>
-      <c r="E14" t="s">
+      <c r="C15" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="D15" t="s">
         <v>447</v>
       </c>
-      <c r="B15" t="s">
+      <c r="E15" t="s">
         <v>448</v>
       </c>
-      <c r="C15" t="s">
+      <c r="F15" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>449</v>
       </c>
-      <c r="D15" t="s">
+      <c r="B16" t="s">
         <v>450</v>
       </c>
-      <c r="E15" t="s">
+      <c r="C16" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="D16" t="s">
         <v>452</v>
       </c>
-      <c r="B16" t="s">
+      <c r="E16" t="s">
         <v>453</v>
       </c>
-      <c r="C16" t="s">
+      <c r="F16" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>449</v>
+      </c>
+      <c r="B17" t="s">
+        <v>450</v>
+      </c>
+      <c r="C17" t="s">
         <v>454</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>455</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>452</v>
-      </c>
-      <c r="B17" t="s">
-        <v>453</v>
-      </c>
-      <c r="C17" t="s">
-        <v>457</v>
-      </c>
-      <c r="D17" t="s">
-        <v>458</v>
-      </c>
-      <c r="E17" t="s">
-        <v>459</v>
+      <c r="F17" t="s">
+        <v>527</v>
       </c>
     </row>
   </sheetData>
@@ -3935,8 +4222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F202BC1-BB1A-48E2-AD9A-32FFB97B837A}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection sqref="A1:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3975,291 +4262,342 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2" t="s">
+        <v>458</v>
+      </c>
+      <c r="C2" t="s">
+        <v>459</v>
+      </c>
+      <c r="D2" t="s">
         <v>460</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>461</v>
       </c>
-      <c r="C2" t="s">
-        <v>462</v>
-      </c>
-      <c r="D2" t="s">
-        <v>463</v>
-      </c>
-      <c r="E2" t="s">
-        <v>464</v>
+      <c r="F2" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B3" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="C3" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D3" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="E3" t="s">
-        <v>467</v>
+        <v>464</v>
+      </c>
+      <c r="F3" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>465</v>
+      </c>
+      <c r="B4" t="s">
+        <v>466</v>
+      </c>
+      <c r="C4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D4" t="s">
         <v>468</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>469</v>
       </c>
-      <c r="C4" t="s">
-        <v>470</v>
-      </c>
-      <c r="D4" t="s">
-        <v>471</v>
-      </c>
-      <c r="E4" t="s">
-        <v>472</v>
+      <c r="F4" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B5" t="s">
+        <v>466</v>
+      </c>
+      <c r="C5" t="s">
+        <v>470</v>
+      </c>
+      <c r="D5" t="s">
+        <v>471</v>
+      </c>
+      <c r="E5" t="s">
         <v>469</v>
       </c>
-      <c r="C5" t="s">
-        <v>473</v>
-      </c>
-      <c r="D5" t="s">
-        <v>474</v>
-      </c>
-      <c r="E5" t="s">
-        <v>472</v>
+      <c r="F5" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B6" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="C6" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="D6" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="E6" t="s">
-        <v>477</v>
+        <v>474</v>
+      </c>
+      <c r="F6" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>475</v>
+      </c>
+      <c r="B7" t="s">
+        <v>476</v>
+      </c>
+      <c r="C7" t="s">
+        <v>477</v>
+      </c>
+      <c r="D7" t="s">
         <v>478</v>
       </c>
-      <c r="B7" t="s">
+      <c r="E7" t="s">
         <v>479</v>
       </c>
-      <c r="C7" t="s">
-        <v>480</v>
-      </c>
-      <c r="D7" t="s">
-        <v>481</v>
-      </c>
-      <c r="E7" t="s">
-        <v>482</v>
+      <c r="F7" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B8" t="s">
+        <v>476</v>
+      </c>
+      <c r="C8" t="s">
+        <v>480</v>
+      </c>
+      <c r="D8" t="s">
+        <v>481</v>
+      </c>
+      <c r="E8" t="s">
         <v>479</v>
       </c>
-      <c r="C8" t="s">
-        <v>483</v>
-      </c>
-      <c r="D8" t="s">
-        <v>484</v>
-      </c>
-      <c r="E8" t="s">
-        <v>482</v>
+      <c r="F8" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>482</v>
+      </c>
+      <c r="B9" t="s">
+        <v>483</v>
+      </c>
+      <c r="C9" t="s">
+        <v>484</v>
+      </c>
+      <c r="D9" t="s">
         <v>485</v>
       </c>
-      <c r="B9" t="s">
+      <c r="E9" t="s">
         <v>486</v>
       </c>
-      <c r="C9" t="s">
-        <v>487</v>
-      </c>
-      <c r="D9" t="s">
-        <v>488</v>
-      </c>
-      <c r="E9" t="s">
-        <v>489</v>
+      <c r="F9" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>487</v>
+      </c>
+      <c r="B10" t="s">
+        <v>488</v>
+      </c>
+      <c r="C10" t="s">
+        <v>489</v>
+      </c>
+      <c r="D10" t="s">
         <v>490</v>
       </c>
-      <c r="B10" t="s">
+      <c r="E10" t="s">
         <v>491</v>
       </c>
-      <c r="C10" t="s">
-        <v>492</v>
-      </c>
-      <c r="D10" t="s">
-        <v>493</v>
-      </c>
-      <c r="E10" t="s">
-        <v>494</v>
+      <c r="F10" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="B11" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="C11" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="D11" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="E11" t="s">
-        <v>497</v>
+        <v>494</v>
+      </c>
+      <c r="F11" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>495</v>
+      </c>
+      <c r="B12" t="s">
+        <v>496</v>
+      </c>
+      <c r="C12" t="s">
+        <v>497</v>
+      </c>
+      <c r="D12" t="s">
         <v>498</v>
       </c>
-      <c r="B12" t="s">
+      <c r="E12" t="s">
         <v>499</v>
       </c>
-      <c r="C12" t="s">
-        <v>500</v>
-      </c>
-      <c r="D12" t="s">
-        <v>501</v>
-      </c>
-      <c r="E12" t="s">
-        <v>502</v>
+      <c r="F12" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B13" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="C13" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="D13" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="E13" t="s">
-        <v>505</v>
+        <v>502</v>
+      </c>
+      <c r="F13" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>503</v>
+      </c>
+      <c r="B14" t="s">
+        <v>504</v>
+      </c>
+      <c r="C14" t="s">
+        <v>505</v>
+      </c>
+      <c r="D14" t="s">
         <v>506</v>
       </c>
-      <c r="B14" t="s">
+      <c r="E14" t="s">
         <v>507</v>
       </c>
-      <c r="C14" t="s">
-        <v>508</v>
-      </c>
-      <c r="D14" t="s">
-        <v>509</v>
-      </c>
-      <c r="E14" t="s">
-        <v>510</v>
+      <c r="F14" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B15" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C15" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="D15" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="E15" t="s">
-        <v>513</v>
+        <v>510</v>
+      </c>
+      <c r="F15" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>511</v>
+      </c>
+      <c r="B16" t="s">
+        <v>512</v>
+      </c>
+      <c r="C16" t="s">
+        <v>513</v>
+      </c>
+      <c r="D16" t="s">
         <v>514</v>
       </c>
-      <c r="B16" t="s">
+      <c r="E16" t="s">
         <v>515</v>
       </c>
-      <c r="C16" t="s">
+      <c r="F16" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>516</v>
       </c>
-      <c r="D16" t="s">
+      <c r="B17" t="s">
         <v>517</v>
       </c>
-      <c r="E16" t="s">
+      <c r="C17" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="D17" t="s">
         <v>519</v>
       </c>
-      <c r="B17" t="s">
+      <c r="E17" t="s">
         <v>520</v>
       </c>
-      <c r="C17" t="s">
+      <c r="F17" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>516</v>
+      </c>
+      <c r="B18" t="s">
+        <v>517</v>
+      </c>
+      <c r="C18" t="s">
         <v>521</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>522</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>519</v>
-      </c>
-      <c r="B18" t="s">
-        <v>520</v>
-      </c>
-      <c r="C18" t="s">
-        <v>524</v>
-      </c>
-      <c r="D18" t="s">
-        <v>525</v>
-      </c>
-      <c r="E18" t="s">
-        <v>526</v>
+      <c r="F18" t="s">
+        <v>527</v>
       </c>
     </row>
   </sheetData>

</xml_diff>